<commit_message>
Model cho QĐ, profile của thiết bị, dashboard của hiếu
</commit_message>
<xml_diff>
--- a/QUANGHANH2/excel/CDVT/download/baocaohoatdong.xlsx
+++ b/QUANGHANH2/excel/CDVT/download/baocaohoatdong.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>Mã thiết bị</t>
   </si>
@@ -84,13 +84,28 @@
     <t>Huyndai</t>
   </si>
   <si>
+    <t>10/02/2010</t>
+  </si>
+  <si>
+    <t>02/10/2011</t>
+  </si>
+  <si>
+    <t>02/10/2015</t>
+  </si>
+  <si>
+    <t>02/11/2010</t>
+  </si>
+  <si>
+    <t>20/05/2012</t>
+  </si>
+  <si>
     <t>Đang hoạt động</t>
   </si>
   <si>
     <t>HD270</t>
   </si>
   <si>
-    <t>C</t>
+    <t>A</t>
   </si>
   <si>
     <t>Đường kế toán</t>
@@ -99,18 +114,12 @@
     <t>Ô tô vận tải Hyundai HD270</t>
   </si>
   <si>
-    <t>Đào lò 3</t>
+    <t>Lộ thiên</t>
   </si>
   <si>
     <t>14L-5684</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Lộ thiên</t>
-  </si>
-  <si>
     <t>14M-5655</t>
   </si>
   <si>
@@ -273,18 +282,24 @@
     <t>Hyundai HL770-9S</t>
   </si>
   <si>
+    <t>ST001</t>
+  </si>
+  <si>
+    <t>Băng tải cấp liệu (số 1)</t>
+  </si>
+  <si>
+    <t>Hệ thống sàng tuyển 1,5 triệu tấn/năm</t>
+  </si>
+  <si>
+    <t>Đào lò 2</t>
+  </si>
+  <si>
     <t>ST002</t>
   </si>
   <si>
     <t>Băng tải cấp liệu (số 2)</t>
   </si>
   <si>
-    <t>Hệ thống sàng tuyển 1,5 triệu tấn/năm</t>
-  </si>
-  <si>
-    <t>Đào lò 2</t>
-  </si>
-  <si>
     <t>ST003</t>
   </si>
   <si>
@@ -307,6 +322,12 @@
   </si>
   <si>
     <t>TBA số1:160kva- 6/0,4kv.(khu VP mỏ Ngã hai)</t>
+  </si>
+  <si>
+    <t>TBA003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TBA số2 160kVA - 6/0,4kv (MB +27) </t>
   </si>
   <si>
     <t/>
@@ -797,8 +818,8 @@
       <c r="C2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="0">
-        <v>40219</v>
+      <c r="D2" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E2" s="0">
         <v>20</v>
@@ -806,46 +827,46 @@
       <c r="F2" s="0">
         <v>1.5</v>
       </c>
-      <c r="G2" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H2" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I2" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J2" s="0">
-        <v>41049</v>
+      <c r="G2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K2" s="0">
         <v>365</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M2" s="0">
         <v>20</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>19</v>
@@ -853,8 +874,8 @@
       <c r="C3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="0">
-        <v>40219</v>
+      <c r="D3" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E3" s="0">
         <v>20</v>
@@ -862,391 +883,391 @@
       <c r="F3" s="0">
         <v>1.5</v>
       </c>
-      <c r="G3" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H3" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I3" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J3" s="0">
-        <v>41049</v>
+      <c r="G3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K3" s="0">
         <v>365</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M3" s="0">
         <v>20</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="O3" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="0">
+        <v>20</v>
+      </c>
+      <c r="F4" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="0">
+        <v>365</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="0">
+        <v>20</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="0">
-        <v>40219</v>
-      </c>
-      <c r="E4" s="0">
-        <v>20</v>
-      </c>
-      <c r="F4" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="G4" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H4" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I4" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J4" s="0">
-        <v>41049</v>
-      </c>
-      <c r="K4" s="0">
-        <v>365</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="0">
-        <v>20</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="P4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="R4" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="0">
+        <v>20</v>
+      </c>
+      <c r="F5" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="0">
+        <v>365</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="0">
+        <v>20</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="0">
-        <v>40219</v>
-      </c>
-      <c r="E5" s="0">
-        <v>20</v>
-      </c>
-      <c r="F5" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="G5" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H5" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I5" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J5" s="0">
-        <v>41049</v>
-      </c>
-      <c r="K5" s="0">
-        <v>365</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="0">
-        <v>20</v>
-      </c>
-      <c r="N5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="P5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q5" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="R5" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="D6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="0">
+        <v>20</v>
+      </c>
+      <c r="F6" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="0">
+        <v>365</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="0">
+        <v>20</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="0">
-        <v>40219</v>
-      </c>
-      <c r="E6" s="0">
-        <v>20</v>
-      </c>
-      <c r="F6" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="G6" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H6" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I6" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J6" s="0">
-        <v>41049</v>
-      </c>
-      <c r="K6" s="0">
-        <v>365</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="0">
-        <v>20</v>
-      </c>
-      <c r="N6" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="P6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="0">
+        <v>20</v>
+      </c>
+      <c r="F7" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="0">
+        <v>365</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="0">
+        <v>20</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q7" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="R7" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="0">
-        <v>40219</v>
-      </c>
-      <c r="E7" s="0">
-        <v>20</v>
-      </c>
-      <c r="F7" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="G7" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H7" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I7" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J7" s="0">
-        <v>41049</v>
-      </c>
-      <c r="K7" s="0">
-        <v>365</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" s="0">
-        <v>20</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="P7" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q7" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="R7" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="0">
+        <v>20</v>
+      </c>
+      <c r="F8" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="0">
+        <v>365</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="0">
+        <v>20</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R8" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="0">
-        <v>40219</v>
-      </c>
-      <c r="E8" s="0">
-        <v>20</v>
-      </c>
-      <c r="F8" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="G8" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H8" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I8" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J8" s="0">
-        <v>41049</v>
-      </c>
-      <c r="K8" s="0">
-        <v>365</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="0">
-        <v>20</v>
-      </c>
-      <c r="N8" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="O8" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="P8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q8" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="R8" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="0">
+        <v>20</v>
+      </c>
+      <c r="F9" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="0">
+        <v>365</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="0">
+        <v>20</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="R9" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="0">
-        <v>40219</v>
-      </c>
-      <c r="E9" s="0">
-        <v>20</v>
-      </c>
-      <c r="F9" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="G9" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H9" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I9" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J9" s="0">
-        <v>41049</v>
-      </c>
-      <c r="K9" s="0">
-        <v>365</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="0">
-        <v>20</v>
-      </c>
-      <c r="N9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="O9" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="P9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q9" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="R9" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E10" s="0">
         <v>20</v>
@@ -1254,55 +1275,55 @@
       <c r="F10" s="0">
         <v>1.5</v>
       </c>
-      <c r="G10" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H10" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I10" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J10" s="0">
-        <v>41049</v>
+      <c r="G10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K10" s="0">
         <v>365</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M10" s="0">
         <v>20</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="O10" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="0">
-        <v>40219</v>
+      <c r="D11" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E11" s="0">
         <v>20</v>
@@ -1310,111 +1331,111 @@
       <c r="F11" s="0">
         <v>1.5</v>
       </c>
-      <c r="G11" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H11" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I11" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J11" s="0">
-        <v>41049</v>
+      <c r="G11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K11" s="0">
         <v>365</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M11" s="0">
         <v>20</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="O11" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="0">
+        <v>20</v>
+      </c>
+      <c r="F12" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="0">
+        <v>365</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M12" s="0">
+        <v>20</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q12" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="0">
-        <v>40219</v>
-      </c>
-      <c r="E12" s="0">
-        <v>20</v>
-      </c>
-      <c r="F12" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="G12" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H12" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I12" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J12" s="0">
-        <v>41049</v>
-      </c>
-      <c r="K12" s="0">
-        <v>365</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M12" s="0">
-        <v>20</v>
-      </c>
-      <c r="N12" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="O12" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="P12" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q12" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="R12" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E13" s="0">
         <v>20</v>
@@ -1422,167 +1443,167 @@
       <c r="F13" s="0">
         <v>1.5</v>
       </c>
-      <c r="G13" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H13" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I13" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J13" s="0">
-        <v>41049</v>
+      <c r="G13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K13" s="0">
         <v>365</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M13" s="0">
         <v>20</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="O13" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q13" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="0">
+        <v>20</v>
+      </c>
+      <c r="F14" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="0">
+        <v>365</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M14" s="0">
+        <v>20</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q14" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="0">
-        <v>40219</v>
-      </c>
-      <c r="E14" s="0">
-        <v>20</v>
-      </c>
-      <c r="F14" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="G14" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H14" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I14" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J14" s="0">
-        <v>41049</v>
-      </c>
-      <c r="K14" s="0">
-        <v>365</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" s="0">
-        <v>20</v>
-      </c>
-      <c r="N14" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="O14" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="P14" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q14" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="R14" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="0">
+        <v>20</v>
+      </c>
+      <c r="F15" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="0">
+        <v>365</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" s="0">
+        <v>20</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q15" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="R15" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="0">
-        <v>40219</v>
-      </c>
-      <c r="E15" s="0">
-        <v>20</v>
-      </c>
-      <c r="F15" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="G15" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H15" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I15" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J15" s="0">
-        <v>41049</v>
-      </c>
-      <c r="K15" s="0">
-        <v>365</v>
-      </c>
-      <c r="L15" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M15" s="0">
-        <v>20</v>
-      </c>
-      <c r="N15" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="O15" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="P15" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q15" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="R15" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E16" s="0">
         <v>20</v>
@@ -1590,55 +1611,55 @@
       <c r="F16" s="0">
         <v>1.5</v>
       </c>
-      <c r="G16" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H16" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I16" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J16" s="0">
-        <v>41049</v>
+      <c r="G16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K16" s="0">
         <v>365</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M16" s="0">
         <v>20</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="O16" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q16" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="R16" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E17" s="0">
         <v>20</v>
@@ -1646,55 +1667,55 @@
       <c r="F17" s="0">
         <v>1.5</v>
       </c>
-      <c r="G17" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H17" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I17" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J17" s="0">
-        <v>41049</v>
+      <c r="G17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K17" s="0">
         <v>365</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M17" s="0">
         <v>20</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="O17" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P17" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q17" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="R17" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E18" s="0">
         <v>20</v>
@@ -1702,55 +1723,55 @@
       <c r="F18" s="0">
         <v>1.5</v>
       </c>
-      <c r="G18" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H18" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I18" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J18" s="0">
-        <v>41049</v>
+      <c r="G18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K18" s="0">
         <v>365</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M18" s="0">
         <v>20</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="O18" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P18" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q18" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="R18" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E19" s="0">
         <v>20</v>
@@ -1758,111 +1779,111 @@
       <c r="F19" s="0">
         <v>1.5</v>
       </c>
-      <c r="G19" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H19" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I19" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J19" s="0">
-        <v>41049</v>
+      <c r="G19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K19" s="0">
         <v>365</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M19" s="0">
         <v>20</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="O19" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P19" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q19" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="R19" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="0">
+        <v>20</v>
+      </c>
+      <c r="F20" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="0">
+        <v>365</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M20" s="0">
+        <v>20</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O20" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q20" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="0">
-        <v>40219</v>
-      </c>
-      <c r="E20" s="0">
-        <v>20</v>
-      </c>
-      <c r="F20" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="G20" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H20" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I20" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J20" s="0">
-        <v>41049</v>
-      </c>
-      <c r="K20" s="0">
-        <v>365</v>
-      </c>
-      <c r="L20" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M20" s="0">
-        <v>20</v>
-      </c>
-      <c r="N20" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="O20" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="P20" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q20" s="0" t="s">
-        <v>61</v>
-      </c>
       <c r="R20" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E21" s="0">
         <v>20</v>
@@ -1870,55 +1891,55 @@
       <c r="F21" s="0">
         <v>1.5</v>
       </c>
-      <c r="G21" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H21" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I21" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J21" s="0">
-        <v>41049</v>
+      <c r="G21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K21" s="0">
         <v>365</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M21" s="0">
         <v>16</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="O21" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P21" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q21" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="R21" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E22" s="0">
         <v>20</v>
@@ -1926,55 +1947,55 @@
       <c r="F22" s="0">
         <v>1.5</v>
       </c>
-      <c r="G22" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H22" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I22" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J22" s="0">
-        <v>41049</v>
+      <c r="G22" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K22" s="0">
         <v>365</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M22" s="0">
         <v>16</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="O22" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P22" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q22" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="R22" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E23" s="0">
         <v>20</v>
@@ -1982,55 +2003,55 @@
       <c r="F23" s="0">
         <v>1.5</v>
       </c>
-      <c r="G23" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H23" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I23" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J23" s="0">
-        <v>41049</v>
+      <c r="G23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K23" s="0">
         <v>365</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M23" s="0">
         <v>16</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="O23" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P23" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q23" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="R23" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E24" s="0">
         <v>20</v>
@@ -2038,55 +2059,55 @@
       <c r="F24" s="0">
         <v>1.5</v>
       </c>
-      <c r="G24" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H24" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I24" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J24" s="0">
-        <v>41049</v>
+      <c r="G24" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K24" s="0">
         <v>365</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M24" s="0">
         <v>16</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="O24" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P24" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q24" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="R24" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E25" s="0">
         <v>20</v>
@@ -2094,55 +2115,55 @@
       <c r="F25" s="0">
         <v>1.5</v>
       </c>
-      <c r="G25" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H25" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I25" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J25" s="0">
-        <v>41049</v>
+      <c r="G25" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K25" s="0">
         <v>365</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M25" s="0">
         <v>16</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="O25" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P25" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q25" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="R25" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E26" s="0">
         <v>20</v>
@@ -2150,55 +2171,55 @@
       <c r="F26" s="0">
         <v>1.5</v>
       </c>
-      <c r="G26" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H26" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I26" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J26" s="0">
-        <v>41049</v>
+      <c r="G26" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K26" s="0">
         <v>365</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M26" s="0">
         <v>16</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="O26" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P26" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q26" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="R26" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E27" s="0">
         <v>20</v>
@@ -2206,55 +2227,55 @@
       <c r="F27" s="0">
         <v>1.5</v>
       </c>
-      <c r="G27" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H27" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I27" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J27" s="0">
-        <v>41049</v>
+      <c r="G27" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K27" s="0">
         <v>365</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M27" s="0">
         <v>16</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="O27" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P27" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q27" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="R27" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E28" s="0">
         <v>20</v>
@@ -2262,55 +2283,55 @@
       <c r="F28" s="0">
         <v>1.5</v>
       </c>
-      <c r="G28" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H28" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I28" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J28" s="0">
-        <v>41049</v>
+      <c r="G28" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K28" s="0">
         <v>365</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M28" s="0">
         <v>16</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="O28" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P28" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q28" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="R28" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E29" s="0">
         <v>20</v>
@@ -2318,167 +2339,167 @@
       <c r="F29" s="0">
         <v>1.5</v>
       </c>
-      <c r="G29" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H29" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I29" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J29" s="0">
-        <v>41049</v>
+      <c r="G29" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K29" s="0">
         <v>365</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M29" s="0">
         <v>20</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="O29" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P29" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q29" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="R29" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B30" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="0">
+        <v>20</v>
+      </c>
+      <c r="F30" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K30" s="0">
+        <v>365</v>
+      </c>
+      <c r="L30" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M30" s="0">
+        <v>20</v>
+      </c>
+      <c r="N30" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O30" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P30" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q30" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="C30" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="0">
-        <v>40219</v>
-      </c>
-      <c r="E30" s="0">
-        <v>20</v>
-      </c>
-      <c r="F30" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="G30" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H30" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I30" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J30" s="0">
-        <v>41049</v>
-      </c>
-      <c r="K30" s="0">
-        <v>365</v>
-      </c>
-      <c r="L30" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M30" s="0">
-        <v>20</v>
-      </c>
-      <c r="N30" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="O30" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="P30" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q30" s="0" t="s">
-        <v>86</v>
-      </c>
       <c r="R30" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="0">
+        <v>20</v>
+      </c>
+      <c r="F31" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K31" s="0">
+        <v>365</v>
+      </c>
+      <c r="L31" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M31" s="0">
+        <v>20</v>
+      </c>
+      <c r="N31" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O31" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P31" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q31" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="R31" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" s="0">
-        <v>40219</v>
-      </c>
-      <c r="E31" s="0">
-        <v>20</v>
-      </c>
-      <c r="F31" s="0">
-        <v>1.5</v>
-      </c>
-      <c r="G31" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H31" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I31" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J31" s="0">
-        <v>41049</v>
-      </c>
-      <c r="K31" s="0">
-        <v>365</v>
-      </c>
-      <c r="L31" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M31" s="0">
-        <v>20</v>
-      </c>
-      <c r="N31" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="O31" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="P31" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q31" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="R31" s="0" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D32" s="0">
-        <v>40219</v>
+        <v>44</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="E32" s="0">
         <v>20</v>
@@ -2486,306 +2507,365 @@
       <c r="F32" s="0">
         <v>1.5</v>
       </c>
-      <c r="G32" s="0">
-        <v>40818</v>
-      </c>
-      <c r="H32" s="0">
-        <v>42279</v>
-      </c>
-      <c r="I32" s="0">
-        <v>40484</v>
-      </c>
-      <c r="J32" s="0">
-        <v>41049</v>
+      <c r="G32" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="K32" s="0">
         <v>365</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M32" s="0">
         <v>20</v>
       </c>
       <c r="N32" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="O32" s="0" t="s">
         <v>28</v>
       </c>
       <c r="P32" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q32" s="0" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="R32" s="0" t="s">
-        <v>93</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="0">
+        <v>20</v>
+      </c>
+      <c r="F33" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K33" s="0">
+        <v>365</v>
+      </c>
+      <c r="L33" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M33" s="0">
+        <v>20</v>
+      </c>
+      <c r="N33" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O33" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P33" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q33" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="R33" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>96</v>
+        <v>21</v>
+      </c>
+      <c r="E34" s="0">
+        <v>20</v>
+      </c>
+      <c r="F34" s="0">
+        <v>1.5</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="K34" s="0" t="s">
-        <v>96</v>
+        <v>25</v>
+      </c>
+      <c r="K34" s="0">
+        <v>365</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>96</v>
+        <v>26</v>
+      </c>
+      <c r="M34" s="0">
+        <v>20</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="O34" s="0" t="s">
-        <v>96</v>
+        <v>28</v>
       </c>
       <c r="P34" s="0" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="Q34" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="R34" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="N35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="O35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="P35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="R35" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="N36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="O36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="P36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="R36" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="L37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="N37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="O37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="P37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="R37" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="K38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="L38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="N38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="O38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="P38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="Q38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="R38" s="0" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>